<commit_message>
Andrew | Added Recalls 573.6 and 573.7 reporting.
</commit_message>
<xml_diff>
--- a/compliance/Legislation Analysis.xlsx
+++ b/compliance/Legislation Analysis.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewhetzler/Documents/Documents - Andrew’s Money Maker/School/DISSERTATION/GitHub/dissertation/compliance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7238E0CA-F0E0-DE43-B4C1-D5107495AB14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DE6A281-0A5E-C34C-AC34-1A99E3C4E8FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6460" yWindow="3800" windowWidth="28040" windowHeight="17440" xr2:uid="{E5CECD30-7D37-2B4A-8954-83C96D258B13}"/>
+    <workbookView xWindow="100" yWindow="500" windowWidth="40860" windowHeight="24400" activeTab="1" xr2:uid="{E5CECD30-7D37-2B4A-8954-83C96D258B13}"/>
   </bookViews>
   <sheets>
     <sheet name="FMVSS Certification" sheetId="1" r:id="rId1"/>
-    <sheet name="Recalls" sheetId="2" r:id="rId2"/>
+    <sheet name="Recalls - Reporting - 573.6" sheetId="2" r:id="rId2"/>
+    <sheet name="Recalls - Reporting - 573.7" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="164">
   <si>
     <t>Attribute</t>
   </si>
@@ -60,9 +61,6 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>567.4(g )(1)</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -78,9 +76,6 @@
     <t>Month of Manufacture</t>
   </si>
   <si>
-    <t>567.4(g )(2)</t>
-  </si>
-  <si>
     <t>1. Allowed values include numerical (e.g., 6) or spelled out (e.,g., June)</t>
   </si>
   <si>
@@ -93,232 +88,448 @@
     <t>Gross Vehicle Weight Rating (GVWR)</t>
   </si>
   <si>
-    <t>567.4(g)(3)</t>
-  </si>
-  <si>
     <t>1. Value must be in pounds</t>
   </si>
   <si>
     <t>Gross Axle Weight Rating (GAWR)</t>
   </si>
   <si>
-    <t>567.4(g)(4)</t>
-  </si>
-  <si>
     <t>1. Value must be in pounds. 2. Must be a value per axle starting from front to rear. 3. Must include tires. See page 277</t>
   </si>
   <si>
     <t>Conformity to Standards Statement</t>
   </si>
   <si>
-    <t>567.4(g)(5)</t>
-  </si>
-  <si>
     <t>1. Must be 1 of 4 values</t>
   </si>
   <si>
     <t>Vehicle Identification Number</t>
   </si>
   <si>
-    <t>567.4(g)(6)</t>
-  </si>
-  <si>
     <t>Type Classification</t>
   </si>
   <si>
-    <t>567.4(g)(7)</t>
-  </si>
-  <si>
     <t>1. Must be  a value from 571.3</t>
   </si>
   <si>
     <t>Multiple GVWR or GAWR</t>
   </si>
   <si>
-    <t>567.4(h)</t>
-  </si>
-  <si>
     <t>1. Manufacturer can optionally list multiple values if they offer different tire sizes. 2. May list addition GVWR / GAWR values at reduced speeds</t>
   </si>
   <si>
     <t>Documentation Tables</t>
   </si>
   <si>
-    <t>567.4(j)</t>
-  </si>
-  <si>
     <t>Model Year</t>
   </si>
   <si>
     <t>Imported Motor Vehicles (Separate Label)</t>
   </si>
   <si>
-    <t>567.4(k)(4)(i)</t>
-  </si>
-  <si>
     <t>1. Model year (if applicable) otherwise year of manufacturer. 2. Line of vehicle</t>
   </si>
   <si>
     <t>Name of Importer</t>
   </si>
   <si>
-    <t>567.4(k)(4)(ii)</t>
-  </si>
-  <si>
     <t>1. Must be spelled out except for Co. and Inc. 2. Preceded by "Imported By".</t>
   </si>
   <si>
     <t>1. Name must be fully spelled out except Co. or Inc. 2. Preceded by "Manufactured by" or "Mfd By"</t>
   </si>
   <si>
-    <t>567.4(k)(4)(iii)</t>
-  </si>
-  <si>
     <t>VIN Compliance</t>
   </si>
   <si>
-    <t>567.4(l)(1) and (2)</t>
-  </si>
-  <si>
     <t>1. If VIN doesn't comply with 49 CFR 565.4 (b), then this value must provide the OEM's identification number</t>
   </si>
   <si>
     <t>Incomplete Vehicle Manufacturers</t>
   </si>
   <si>
-    <t>567.5(b)(2)(i)</t>
-  </si>
-  <si>
     <t>1. Preceded by "incomplete vehicle MANUFACTURED BY"</t>
   </si>
   <si>
-    <t>567.5(b)(2)(ii)</t>
-  </si>
-  <si>
-    <t>567.5(b)(2)(iii)</t>
-  </si>
-  <si>
     <t>1. Value must be in kilograms and pounds.</t>
   </si>
   <si>
-    <t>567.5(b)(2)(iv)</t>
-  </si>
-  <si>
     <t>1. Value must be in kilograms and pounds. 2. Must be a value per axle starting from front to rear</t>
   </si>
   <si>
-    <t>567.5(b)(2)(v)</t>
-  </si>
-  <si>
     <t>Intermediate Vehicle Manufacturers</t>
   </si>
   <si>
-    <t>567.5(c)(2)(i)</t>
-  </si>
-  <si>
     <t xml:space="preserve">1. Value must be preceded by "INTERMEDIATE MANUFACTURE BY" </t>
   </si>
   <si>
-    <t>567.5(c)(2)(ii)</t>
-  </si>
-  <si>
-    <t>567.5(c)(2)(iii)</t>
-  </si>
-  <si>
     <t>1. Only required if different from the incomplete manufacturer</t>
   </si>
   <si>
-    <t>567.5(c)(2)(iv)</t>
-  </si>
-  <si>
-    <t>567.5(c)(2)(v)</t>
-  </si>
-  <si>
     <t>Final-stage Manufacturers</t>
   </si>
   <si>
-    <t>567.5(d)(2)(i)</t>
-  </si>
-  <si>
     <t>1. Value must be preceded by "MANUFACTURED BY"</t>
   </si>
   <si>
-    <t>567.5(d)(2)(ii)</t>
-  </si>
-  <si>
-    <t>567.5(d)(2)(iii)</t>
-  </si>
-  <si>
-    <t>567.5(d)(2)(iv)</t>
-  </si>
-  <si>
     <t>1. Value must be in kilograms and pounds. 2. Must be in order from front to rear.</t>
   </si>
   <si>
-    <t>567.5(d)(2)(v)</t>
-  </si>
-  <si>
     <t>1. Must be 1 of 3 values</t>
   </si>
   <si>
-    <t>567.5(d)(2)(vi)</t>
-  </si>
-  <si>
-    <t>567.5(d)(2)(vii)</t>
-  </si>
-  <si>
     <t>Altered Certiffied Vehicle Manufacturers</t>
   </si>
   <si>
-    <t>567.7(b)(1)</t>
-  </si>
-  <si>
-    <t>567.5 (e )</t>
-  </si>
-  <si>
-    <t>567.7(b)(2)</t>
-  </si>
-  <si>
     <t>1. Only required if the value changed from the original certification.</t>
   </si>
   <si>
-    <t>567.7(b)(3)</t>
-  </si>
-  <si>
-    <t>567.8(e )(1)</t>
-  </si>
-  <si>
     <t>Replica Vehicle Manufacturers</t>
   </si>
   <si>
-    <t>567.8(e )(2)</t>
-  </si>
-  <si>
-    <t>567.8(e )(3)</t>
-  </si>
-  <si>
-    <t>567.8(e )(4)</t>
-  </si>
-  <si>
     <t xml:space="preserve">1. Value must be in pounds. 2. Must be a value per axle starting from front to rear. </t>
   </si>
   <si>
     <t>Replica Statement</t>
   </si>
   <si>
-    <t>567.8(e )(5)</t>
-  </si>
-  <si>
     <t>Exemption Statement</t>
   </si>
   <si>
-    <t>567.8(e )(6)</t>
-  </si>
-  <si>
     <t>1. Must be 1 of 2 values.</t>
   </si>
   <si>
-    <t>567.8(e )(7)</t>
+    <t>Applies to manufacturers of complete vehicles, incomplete vehicles, and original/replacement equipment 49 CFR 573.3(a)</t>
+  </si>
+  <si>
+    <t>ATTRIBUTE</t>
+  </si>
+  <si>
+    <t>REQUIRED</t>
+  </si>
+  <si>
+    <t>CITATION</t>
+  </si>
+  <si>
+    <t>NOTES</t>
+  </si>
+  <si>
+    <t>49 CFR 567.4(g )(1)</t>
+  </si>
+  <si>
+    <t>49 CFR 567.4(g )(2)</t>
+  </si>
+  <si>
+    <t>49 CFR 567.4(g)(3)</t>
+  </si>
+  <si>
+    <t>49 CFR 567.4(g)(4)</t>
+  </si>
+  <si>
+    <t>49 CFR 567.4(g)(5)</t>
+  </si>
+  <si>
+    <t>49 CFR 567.4(g)(6)</t>
+  </si>
+  <si>
+    <t>49 CFR 567.4(g)(7)</t>
+  </si>
+  <si>
+    <t>49 CFR 567.4(h)</t>
+  </si>
+  <si>
+    <t>49 CFR 567.4(j)</t>
+  </si>
+  <si>
+    <t>49 CFR 567.4(k)(4)(i)</t>
+  </si>
+  <si>
+    <t>49 CFR 567.4(k)(4)(ii)</t>
+  </si>
+  <si>
+    <t>49 CFR 567.4(k)(4)(iii)</t>
+  </si>
+  <si>
+    <t>49 CFR 567.4(l)(1) and (2)</t>
+  </si>
+  <si>
+    <t>49 CFR 567.5(b)(2)(i)</t>
+  </si>
+  <si>
+    <t>49 CFR 567.5(b)(2)(ii)</t>
+  </si>
+  <si>
+    <t>49 CFR 567.5(b)(2)(iii)</t>
+  </si>
+  <si>
+    <t>49 CFR 567.5(b)(2)(iv)</t>
+  </si>
+  <si>
+    <t>49 CFR 567.5(b)(2)(v)</t>
+  </si>
+  <si>
+    <t>49 CFR 567.5(c)(2)(i)</t>
+  </si>
+  <si>
+    <t>49 CFR 567.5(c)(2)(ii)</t>
+  </si>
+  <si>
+    <t>49 CFR 567.5(c)(2)(iii)</t>
+  </si>
+  <si>
+    <t>49 CFR 567.5(c)(2)(iv)</t>
+  </si>
+  <si>
+    <t>49 CFR 567.5(c)(2)(v)</t>
+  </si>
+  <si>
+    <t>49 CFR 567.5(d)(2)(i)</t>
+  </si>
+  <si>
+    <t>49 CFR 567.5(d)(2)(ii)</t>
+  </si>
+  <si>
+    <t>49 CFR 567.5(d)(2)(iii)</t>
+  </si>
+  <si>
+    <t>49 CFR 567.5(d)(2)(iv)</t>
+  </si>
+  <si>
+    <t>49 CFR 567.5(d)(2)(v)</t>
+  </si>
+  <si>
+    <t>49 CFR 567.5(d)(2)(vi)</t>
+  </si>
+  <si>
+    <t>49 CFR 567.5(d)(2)(vii)</t>
+  </si>
+  <si>
+    <t>49 CFR 567.5 (e )</t>
+  </si>
+  <si>
+    <t>49 CFR 567.7(b)(1)</t>
+  </si>
+  <si>
+    <t>49 CFR 567.7(b)(2)</t>
+  </si>
+  <si>
+    <t>49 CFR 567.7(b)(3)</t>
+  </si>
+  <si>
+    <t>49 CFR 567.8(e )(1)</t>
+  </si>
+  <si>
+    <t>49 CFR 567.8(e )(2)</t>
+  </si>
+  <si>
+    <t>49 CFR 567.8(e )(3)</t>
+  </si>
+  <si>
+    <t>49 CFR 567.8(e )(4)</t>
+  </si>
+  <si>
+    <t>49 CFR 567.8(e )(5)</t>
+  </si>
+  <si>
+    <t>49 CFR 567.8(e )(6)</t>
+  </si>
+  <si>
+    <t>49 CFR 567.8(e )(7)</t>
+  </si>
+  <si>
+    <t>1. Full company name and any brand name/trademark owner. Must be spelled out except for Co or Inc. 2. For imported cars, the designated agency by the fabricating manufacturer should also be listed.</t>
+  </si>
+  <si>
+    <t>49 CFR 573.6 (c) (1)</t>
+  </si>
+  <si>
+    <t>Identification of Vehicles</t>
+  </si>
+  <si>
+    <t>Identification of Equipment</t>
+  </si>
+  <si>
+    <t>49 CFR 573.6 (c) (2)</t>
+  </si>
+  <si>
+    <t>Description of Basis for Determination of Recall Population</t>
+  </si>
+  <si>
+    <t>Description of Vehicles or Equipment Differ From Similar Vehicles/Equipment Not Included in Recall</t>
+  </si>
+  <si>
+    <t>1. Note that the statute says it must be either id of vehicles OR equipment. 2. For passenger cars, id is the make, line, model year, inclusive dates (month + year) of manufacture, other info needed to describe vehicles ((2)(i)). 3. For other cars, id is body style/type, inclusive dates of manufacture, other info needed to describe vehicles (GVWR or class for trucks, displacement for motorcycles, # of passengers for bus) ((2)(ii)).4.  If vehicle/component manufactured by a different manufacturer, the reporting manufacturer identifies the origin country, name of manufacturer and/or assembler, business address, business telephone # (2)(iv)</t>
+  </si>
+  <si>
+    <t>1. Note that the statute says it must be either id of vehicles OR equipment. 2. For items, id is the generic name of the component, part #s, size and function (if applicable), inclusive dates of manufacture (if available), brand, model name, model number (as applicable), and other details needed. 3. If vehicle/component manufactured by a different manufacturer, the reporting manufacturer identifies the origin country, name of manufacturer and/or assembler, business address, business telephone # (2)(iv). 4. For items of motor vehicle equipment, the manufacturer of equipment identify by name, business address, business telephone # every manufacturer that purchases defective/noncompliant items for use or install in new vehicles or new item of equipment (2)(v)</t>
+  </si>
+  <si>
+    <t>Total Number of Vehicles/Equipment Potentially Containing Defect/NonCompliance</t>
+  </si>
+  <si>
+    <t>49 CFR 573.6 (c) (3)</t>
+  </si>
+  <si>
+    <t>1. Where available, the # of vehicles/items in each group identified in paragraph (c ) (2)</t>
+  </si>
+  <si>
+    <t>% of Vehicles/Items Estimated to Contain Defect/Compliance</t>
+  </si>
+  <si>
+    <t>49 CFR 573.6 (c) (4)</t>
+  </si>
+  <si>
+    <t>Description of Defect/Noncompliance</t>
+  </si>
+  <si>
+    <t>49 CFR 573.6 (c) (5)</t>
+  </si>
+  <si>
+    <t>1. Contain a brief  summary and detailed description. 2. Graphic aids as necessary.</t>
+  </si>
+  <si>
+    <t>Identify and Describe Risk to Motor Vehicle Safety</t>
+  </si>
+  <si>
+    <t>Chronology of Principal Events Led to Determination</t>
+  </si>
+  <si>
+    <t>49 CFR 573.6 (c) (6)</t>
+  </si>
+  <si>
+    <t>1. Only applies to defects. 2. Include summary of all warranty claims, field/service reports, other info, with dates of receipt</t>
+  </si>
+  <si>
+    <t>49 CFR 573.6 (c) (7)</t>
+  </si>
+  <si>
+    <t>Test Results</t>
+  </si>
+  <si>
+    <t>1. Only applies to non-compliance. 2. Test results/other info manufacturer considered in determining existence of non-compliance. 3. Id the date of each test and observation that indicated non-compliance might or did exist</t>
+  </si>
+  <si>
+    <t>Manufacturer Remedy Program</t>
+  </si>
+  <si>
+    <t>49 CFR 573.6 (c) (8) (i)</t>
+  </si>
+  <si>
+    <t>Estimated Dates for Notifications To Owners/Dealers/Distributors</t>
+  </si>
+  <si>
+    <t>49 CFR 573.6 (c) (8) (ii)</t>
+  </si>
+  <si>
+    <t>1. Must include beginning and ending dates.</t>
+  </si>
+  <si>
+    <t>49 CFR 573.6 (c) (8) (iii)</t>
+  </si>
+  <si>
+    <t>Petition for Exemption Due to Inconsequential Defect/Non-compliance</t>
+  </si>
+  <si>
+    <t>1. Only if manufacturer plans to file.</t>
+  </si>
+  <si>
+    <t>1. Include a plan for reimbursement 2. Remedy programs need updated every 2 years. 3. Public can view reimbursement and remedy plans @ NHTSA HQ. If remedy program contains tires: address how manufacturer will assure entites replacing tires are aware of legal requirements related to tire recalls; how manufacturer prevents recalled tires from being re-sold: written directions to alter recalled tires; requirement for manufacturer-owned/other manufacturer-controlled outlets report to manufacturer the # of recalled tires removed, how manufacturer will dispose tires: written directions require manufacturer-owned to either (a) ship recalled tires, (b) ship to a location of their choosing; manufacturer-owned/controlled report to manufactuer the # of recalled tires disposed in violation of applicate local/state laws; description of manufacturer's program for disposing recalled tires returned to manufacturer</t>
+  </si>
+  <si>
+    <t>Copy of Notices/Bulletins/Other Communication</t>
+  </si>
+  <si>
+    <t xml:space="preserve">49 CFR 573.6 (c) (10) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">49 CFR 573.6 (c) (11) </t>
+  </si>
+  <si>
+    <t>Manufacter's Campaign #</t>
+  </si>
+  <si>
+    <t>1. Only required if different than the # assigned by the NHTSA</t>
+  </si>
+  <si>
+    <t>Notification Campaign #</t>
+  </si>
+  <si>
+    <t>49 CFR 573.7 (b) (1)</t>
+  </si>
+  <si>
+    <t>This is the quarterly report for manufacturers conducting defect/noncompliance notification campaigns</t>
+  </si>
+  <si>
+    <t>Date Notification Began</t>
+  </si>
+  <si>
+    <t>49 CFR 573.7 (b) (2)</t>
+  </si>
+  <si>
+    <t>Date Notification Completed</t>
+  </si>
+  <si>
+    <t># of Vehicles/Items Involved in Notification</t>
+  </si>
+  <si>
+    <t>49 CFR 573.7 (b) (3)</t>
+  </si>
+  <si>
+    <t># of Vehicles/Equipment  Inspected and Repaired</t>
+  </si>
+  <si>
+    <t>49 CFR 573.7 (b) (4)</t>
+  </si>
+  <si>
+    <t># of Vehicles/Equipment  Inspected and Not Needing Repaired</t>
+  </si>
+  <si>
+    <t># of Vehicles/Equipemnt Determined to be Unreachable</t>
+  </si>
+  <si>
+    <t>49 CFR 573.7 (b) (5)</t>
+  </si>
+  <si>
+    <t>1. There are specific categories: export, theft, scrapping, failure to receive notification, other reasons (must specifiy). 2. The # must be broken out by category</t>
+  </si>
+  <si>
+    <t># of Equipment Repaired/Returned Prior to 1st Sale</t>
+  </si>
+  <si>
+    <t>49 CFR 573.7 (b) (6)</t>
+  </si>
+  <si>
+    <t>Agreegate # of Recalled Tires Manufacturer Becomes Aware Not Rendered Unuitable for Resale</t>
+  </si>
+  <si>
+    <t>49 CFR 573.7 (b) (7) (i)</t>
+  </si>
+  <si>
+    <t>1. Only applies to tires. 2. Is required for tires.</t>
+  </si>
+  <si>
+    <t>1. Only applies to equipment manufacturers. 2. Is required for equipment manufacturers.  3. Equipment must be returned by dealers, other retailers, and distributors to the manufacturer</t>
+  </si>
+  <si>
+    <t>Aggregate # of Manufacturer Aware Disposed of in Violation</t>
+  </si>
+  <si>
+    <t>49 CFR 573.7 (b) (7) (ii)</t>
+  </si>
+  <si>
+    <t>49 CFR 573.7 (b) (7) (iii)</t>
+  </si>
+  <si>
+    <t>Description of Failures of Tire Outlet to Act in Accordance with Directions in Manufacturer's Plan</t>
+  </si>
+  <si>
+    <t>Information suppled in response to (b)(4) and (b)(5) are Cumalative Totals</t>
+  </si>
+  <si>
+    <t>49 CFR 573.7 (b) (7) (iii) ©</t>
+  </si>
+  <si>
+    <t>Defect and noncompliance report</t>
   </si>
 </sst>
 </file>
@@ -368,13 +579,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -711,7 +931,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FB94E3D-C5C3-3841-8945-149F56AC5305}">
   <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
@@ -738,7 +958,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -752,10 +972,10 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>58</v>
       </c>
       <c r="E2" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -763,16 +983,16 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" t="s">
         <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -780,16 +1000,16 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4" t="s">
         <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -797,16 +1017,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -814,16 +1034,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>60</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -831,16 +1051,16 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
+        <v>61</v>
       </c>
       <c r="E7" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -848,16 +1068,16 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>62</v>
       </c>
       <c r="E8" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -865,13 +1085,13 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -879,16 +1099,16 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
         <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
+        <v>64</v>
       </c>
       <c r="E10" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -896,16 +1116,16 @@
         <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>32</v>
+        <v>65</v>
       </c>
       <c r="E11" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -913,83 +1133,83 @@
         <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>35</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C14" t="s">
         <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>38</v>
+        <v>67</v>
       </c>
       <c r="E14" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C15" t="s">
         <v>6</v>
       </c>
       <c r="D15" t="s">
-        <v>41</v>
+        <v>68</v>
       </c>
       <c r="E15" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C16" t="s">
         <v>6</v>
       </c>
       <c r="D16" t="s">
-        <v>44</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B17" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="C17" t="s">
         <v>6</v>
       </c>
       <c r="D17" t="s">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="E17" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="B19" t="s">
         <v>5</v>
@@ -998,97 +1218,97 @@
         <v>6</v>
       </c>
       <c r="D19" t="s">
-        <v>49</v>
+        <v>71</v>
       </c>
       <c r="E19" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="B20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" t="s">
+        <v>72</v>
+      </c>
+      <c r="E20" t="s">
         <v>12</v>
-      </c>
-      <c r="C20" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" t="s">
-        <v>51</v>
-      </c>
-      <c r="E20" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="B21" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C21" t="s">
         <v>6</v>
       </c>
       <c r="D21" t="s">
-        <v>51</v>
+        <v>72</v>
       </c>
       <c r="E21" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="B22" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C22" t="s">
         <v>6</v>
       </c>
       <c r="D22" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
       <c r="E22" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="B23" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C23" t="s">
         <v>6</v>
       </c>
       <c r="D23" t="s">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="E23" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="B24" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C24" t="s">
         <v>6</v>
       </c>
       <c r="D24" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="B25" t="s">
         <v>5</v>
@@ -1097,97 +1317,97 @@
         <v>6</v>
       </c>
       <c r="D25" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="E25" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="B26" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" t="s">
+        <v>77</v>
+      </c>
+      <c r="E26" t="s">
         <v>12</v>
-      </c>
-      <c r="C26" t="s">
-        <v>6</v>
-      </c>
-      <c r="D26" t="s">
-        <v>60</v>
-      </c>
-      <c r="E26" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="B27" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C27" t="s">
         <v>6</v>
       </c>
       <c r="D27" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="E27" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="B28" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C28" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D28" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="E28" t="s">
-        <v>62</v>
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="B29" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D29" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="E29" t="s">
-        <v>62</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="B30" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C30" t="s">
         <v>6</v>
       </c>
       <c r="D30" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="B31" t="s">
         <v>5</v>
@@ -1196,199 +1416,199 @@
         <v>6</v>
       </c>
       <c r="D31" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="E31" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="B32" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E32" t="s">
         <v>12</v>
-      </c>
-      <c r="C32" t="s">
-        <v>6</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E32" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="B33" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C33" t="s">
         <v>6</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="E33" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="B34" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C34" t="s">
         <v>6</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="E34" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="B35" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C35" t="s">
         <v>6</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="E35" t="s">
-        <v>71</v>
+        <v>44</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="B36" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C36" t="s">
         <v>6</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="E36" t="s">
-        <v>73</v>
+        <v>45</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="B37" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C37" t="s">
         <v>6</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="B38" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C38" t="s">
         <v>6</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="B39" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C39" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>76</v>
+        <v>46</v>
       </c>
       <c r="B41" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C41" t="s">
         <v>6</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>76</v>
+        <v>46</v>
       </c>
       <c r="B42" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C42" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="E42" t="s">
-        <v>80</v>
+        <v>47</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>76</v>
+        <v>46</v>
       </c>
       <c r="B43" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C43" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="E43" t="s">
-        <v>80</v>
+        <v>47</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>76</v>
+        <v>46</v>
       </c>
       <c r="B44" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C44" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="E44">
         <v>1</v>
@@ -1396,7 +1616,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>83</v>
+        <v>48</v>
       </c>
       <c r="B46" t="s">
         <v>5</v>
@@ -1405,123 +1625,123 @@
         <v>6</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="E46" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>83</v>
+        <v>48</v>
       </c>
       <c r="B47" t="s">
+        <v>11</v>
+      </c>
+      <c r="C47" t="s">
+        <v>6</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E47" t="s">
         <v>12</v>
-      </c>
-      <c r="C47" t="s">
-        <v>6</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="E47" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>83</v>
+        <v>48</v>
       </c>
       <c r="B48" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C48" t="s">
         <v>6</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="E48" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>83</v>
+        <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C49" t="s">
         <v>6</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="E49" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>83</v>
+        <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C50" t="s">
         <v>6</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="E50" t="s">
-        <v>87</v>
+        <v>49</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>83</v>
+        <v>48</v>
       </c>
       <c r="B51" t="s">
-        <v>88</v>
+        <v>50</v>
       </c>
       <c r="C51" t="s">
         <v>6</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>83</v>
+        <v>48</v>
       </c>
       <c r="B52" t="s">
-        <v>90</v>
+        <v>51</v>
       </c>
       <c r="C52" t="s">
         <v>6</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="E52" t="s">
-        <v>92</v>
+        <v>52</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>83</v>
+        <v>48</v>
       </c>
       <c r="B53" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C53" t="s">
         <v>6</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1531,12 +1751,1573 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A11599B-9DA0-2045-BC7A-DB9B12AD7FC4}">
-  <dimension ref="A1"/>
+  <dimension ref="A2:H315"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="88.5" customWidth="1"/>
+    <col min="2" max="2" width="18.83203125" customWidth="1"/>
+    <col min="3" max="3" width="27.1640625" customWidth="1"/>
+    <col min="4" max="4" width="120" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>100</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="85" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>103</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="102" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>102</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>103</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>104</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>103</v>
+      </c>
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>105</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>103</v>
+      </c>
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>108</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>109</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>112</v>
+      </c>
+      <c r="D12" s="4"/>
+    </row>
+    <row r="13" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>113</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>114</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>116</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>114</v>
+      </c>
+      <c r="D14" s="4"/>
+    </row>
+    <row r="15" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>117</v>
+      </c>
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" t="s">
+        <v>118</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>121</v>
+      </c>
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
+        <v>120</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="119" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>123</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>124</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>125</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" t="s">
+        <v>126</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>129</v>
+      </c>
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" t="s">
+        <v>128</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>132</v>
+      </c>
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D20" s="4"/>
+    </row>
+    <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>135</v>
+      </c>
+      <c r="B21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D22" s="4"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D23" s="4"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D24" s="4"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D25" s="4"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D26" s="4"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D27" s="4"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D28" s="4"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D29" s="4"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D30" s="4"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D31" s="4"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D32" s="4"/>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D33" s="4"/>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D34" s="4"/>
+    </row>
+    <row r="35" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D35" s="4"/>
+    </row>
+    <row r="36" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D36" s="4"/>
+    </row>
+    <row r="37" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D37" s="4"/>
+    </row>
+    <row r="38" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D38" s="4"/>
+    </row>
+    <row r="39" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D39" s="4"/>
+    </row>
+    <row r="40" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D40" s="4"/>
+    </row>
+    <row r="41" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D41" s="4"/>
+    </row>
+    <row r="42" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D42" s="4"/>
+    </row>
+    <row r="43" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D43" s="4"/>
+    </row>
+    <row r="44" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D44" s="4"/>
+    </row>
+    <row r="45" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D45" s="4"/>
+    </row>
+    <row r="46" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D46" s="4"/>
+    </row>
+    <row r="47" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D47" s="4"/>
+    </row>
+    <row r="48" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D48" s="4"/>
+    </row>
+    <row r="49" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D49" s="4"/>
+    </row>
+    <row r="50" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D50" s="4"/>
+    </row>
+    <row r="51" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D51" s="4"/>
+    </row>
+    <row r="52" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D52" s="4"/>
+    </row>
+    <row r="53" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D53" s="4"/>
+    </row>
+    <row r="54" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D54" s="4"/>
+    </row>
+    <row r="55" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D55" s="4"/>
+    </row>
+    <row r="56" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D56" s="4"/>
+    </row>
+    <row r="57" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D57" s="4"/>
+    </row>
+    <row r="58" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D58" s="4"/>
+    </row>
+    <row r="59" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D59" s="4"/>
+    </row>
+    <row r="60" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D60" s="4"/>
+    </row>
+    <row r="61" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D61" s="4"/>
+    </row>
+    <row r="62" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D62" s="4"/>
+    </row>
+    <row r="63" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D63" s="4"/>
+    </row>
+    <row r="64" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D64" s="4"/>
+    </row>
+    <row r="65" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D65" s="4"/>
+    </row>
+    <row r="66" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D66" s="5"/>
+    </row>
+    <row r="67" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D67" s="5"/>
+    </row>
+    <row r="68" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D68" s="5"/>
+    </row>
+    <row r="69" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D69" s="5"/>
+    </row>
+    <row r="70" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D70" s="5"/>
+    </row>
+    <row r="71" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D71" s="5"/>
+    </row>
+    <row r="72" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D72" s="5"/>
+    </row>
+    <row r="73" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D73" s="5"/>
+    </row>
+    <row r="74" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D74" s="5"/>
+    </row>
+    <row r="75" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D75" s="5"/>
+    </row>
+    <row r="76" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D76" s="5"/>
+    </row>
+    <row r="77" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D77" s="5"/>
+    </row>
+    <row r="78" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D78" s="5"/>
+    </row>
+    <row r="79" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D79" s="5"/>
+    </row>
+    <row r="80" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D80" s="5"/>
+    </row>
+    <row r="81" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D81" s="5"/>
+    </row>
+    <row r="82" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D82" s="5"/>
+    </row>
+    <row r="83" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D83" s="5"/>
+    </row>
+    <row r="84" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D84" s="5"/>
+    </row>
+    <row r="85" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D85" s="5"/>
+    </row>
+    <row r="86" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D86" s="5"/>
+    </row>
+    <row r="87" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D87" s="5"/>
+    </row>
+    <row r="88" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D88" s="5"/>
+    </row>
+    <row r="89" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D89" s="5"/>
+    </row>
+    <row r="90" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D90" s="5"/>
+    </row>
+    <row r="91" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D91" s="5"/>
+    </row>
+    <row r="92" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D92" s="5"/>
+    </row>
+    <row r="93" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D93" s="5"/>
+    </row>
+    <row r="94" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D94" s="5"/>
+    </row>
+    <row r="95" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D95" s="5"/>
+    </row>
+    <row r="96" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D96" s="5"/>
+    </row>
+    <row r="97" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D97" s="5"/>
+    </row>
+    <row r="98" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D98" s="5"/>
+    </row>
+    <row r="99" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D99" s="5"/>
+    </row>
+    <row r="100" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D100" s="5"/>
+    </row>
+    <row r="101" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D101" s="5"/>
+    </row>
+    <row r="102" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D102" s="5"/>
+    </row>
+    <row r="103" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D103" s="5"/>
+    </row>
+    <row r="104" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D104" s="5"/>
+    </row>
+    <row r="105" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D105" s="5"/>
+    </row>
+    <row r="106" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D106" s="5"/>
+    </row>
+    <row r="107" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D107" s="5"/>
+    </row>
+    <row r="108" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D108" s="5"/>
+    </row>
+    <row r="109" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D109" s="5"/>
+    </row>
+    <row r="110" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D110" s="5"/>
+    </row>
+    <row r="111" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D111" s="5"/>
+    </row>
+    <row r="112" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D112" s="5"/>
+    </row>
+    <row r="113" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D113" s="5"/>
+    </row>
+    <row r="114" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D114" s="5"/>
+    </row>
+    <row r="115" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D115" s="5"/>
+    </row>
+    <row r="116" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D116" s="5"/>
+    </row>
+    <row r="117" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D117" s="5"/>
+    </row>
+    <row r="118" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D118" s="5"/>
+    </row>
+    <row r="119" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D119" s="5"/>
+    </row>
+    <row r="120" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D120" s="5"/>
+    </row>
+    <row r="121" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D121" s="5"/>
+    </row>
+    <row r="122" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D122" s="5"/>
+    </row>
+    <row r="123" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D123" s="5"/>
+    </row>
+    <row r="124" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D124" s="5"/>
+    </row>
+    <row r="125" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D125" s="5"/>
+    </row>
+    <row r="126" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D126" s="5"/>
+    </row>
+    <row r="127" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D127" s="5"/>
+    </row>
+    <row r="128" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D128" s="5"/>
+    </row>
+    <row r="129" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D129" s="5"/>
+    </row>
+    <row r="130" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D130" s="5"/>
+    </row>
+    <row r="131" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D131" s="5"/>
+    </row>
+    <row r="132" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D132" s="5"/>
+    </row>
+    <row r="133" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D133" s="5"/>
+    </row>
+    <row r="134" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D134" s="5"/>
+    </row>
+    <row r="135" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D135" s="5"/>
+    </row>
+    <row r="136" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D136" s="5"/>
+    </row>
+    <row r="137" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D137" s="5"/>
+    </row>
+    <row r="138" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D138" s="5"/>
+    </row>
+    <row r="139" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D139" s="5"/>
+    </row>
+    <row r="140" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D140" s="5"/>
+    </row>
+    <row r="141" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D141" s="5"/>
+    </row>
+    <row r="142" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D142" s="5"/>
+    </row>
+    <row r="143" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D143" s="5"/>
+    </row>
+    <row r="144" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D144" s="5"/>
+    </row>
+    <row r="145" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D145" s="5"/>
+    </row>
+    <row r="146" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D146" s="5"/>
+    </row>
+    <row r="147" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D147" s="5"/>
+    </row>
+    <row r="148" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D148" s="5"/>
+    </row>
+    <row r="149" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D149" s="5"/>
+    </row>
+    <row r="150" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D150" s="5"/>
+    </row>
+    <row r="151" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D151" s="5"/>
+    </row>
+    <row r="152" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D152" s="5"/>
+    </row>
+    <row r="153" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D153" s="5"/>
+    </row>
+    <row r="154" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D154" s="5"/>
+    </row>
+    <row r="155" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D155" s="5"/>
+    </row>
+    <row r="156" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D156" s="5"/>
+    </row>
+    <row r="157" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D157" s="5"/>
+    </row>
+    <row r="158" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D158" s="5"/>
+    </row>
+    <row r="159" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D159" s="5"/>
+    </row>
+    <row r="160" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D160" s="5"/>
+    </row>
+    <row r="161" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D161" s="5"/>
+    </row>
+    <row r="162" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D162" s="5"/>
+    </row>
+    <row r="163" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D163" s="5"/>
+    </row>
+    <row r="164" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D164" s="5"/>
+    </row>
+    <row r="165" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D165" s="5"/>
+    </row>
+    <row r="166" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D166" s="5"/>
+    </row>
+    <row r="167" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D167" s="5"/>
+    </row>
+    <row r="168" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D168" s="5"/>
+    </row>
+    <row r="169" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D169" s="5"/>
+    </row>
+    <row r="170" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D170" s="5"/>
+    </row>
+    <row r="171" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D171" s="5"/>
+    </row>
+    <row r="172" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D172" s="5"/>
+    </row>
+    <row r="173" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D173" s="5"/>
+    </row>
+    <row r="174" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D174" s="5"/>
+    </row>
+    <row r="175" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D175" s="5"/>
+    </row>
+    <row r="176" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D176" s="5"/>
+    </row>
+    <row r="177" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D177" s="5"/>
+    </row>
+    <row r="178" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D178" s="5"/>
+    </row>
+    <row r="179" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D179" s="5"/>
+    </row>
+    <row r="180" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D180" s="5"/>
+    </row>
+    <row r="181" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D181" s="5"/>
+    </row>
+    <row r="182" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D182" s="5"/>
+    </row>
+    <row r="183" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D183" s="5"/>
+    </row>
+    <row r="184" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D184" s="5"/>
+    </row>
+    <row r="185" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D185" s="5"/>
+    </row>
+    <row r="186" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D186" s="5"/>
+    </row>
+    <row r="187" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D187" s="5"/>
+    </row>
+    <row r="188" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D188" s="5"/>
+    </row>
+    <row r="189" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D189" s="5"/>
+    </row>
+    <row r="190" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D190" s="5"/>
+    </row>
+    <row r="191" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D191" s="5"/>
+    </row>
+    <row r="192" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D192" s="5"/>
+    </row>
+    <row r="193" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D193" s="5"/>
+    </row>
+    <row r="194" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D194" s="5"/>
+    </row>
+    <row r="195" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D195" s="5"/>
+    </row>
+    <row r="196" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D196" s="5"/>
+    </row>
+    <row r="197" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D197" s="5"/>
+    </row>
+    <row r="198" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D198" s="5"/>
+    </row>
+    <row r="199" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D199" s="5"/>
+    </row>
+    <row r="200" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D200" s="5"/>
+    </row>
+    <row r="201" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D201" s="5"/>
+    </row>
+    <row r="202" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D202" s="5"/>
+    </row>
+    <row r="203" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D203" s="5"/>
+    </row>
+    <row r="204" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D204" s="5"/>
+    </row>
+    <row r="205" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D205" s="5"/>
+    </row>
+    <row r="206" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D206" s="5"/>
+    </row>
+    <row r="207" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D207" s="5"/>
+    </row>
+    <row r="208" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D208" s="5"/>
+    </row>
+    <row r="209" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D209" s="5"/>
+    </row>
+    <row r="210" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D210" s="5"/>
+    </row>
+    <row r="211" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D211" s="5"/>
+    </row>
+    <row r="212" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D212" s="5"/>
+    </row>
+    <row r="213" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D213" s="5"/>
+    </row>
+    <row r="214" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D214" s="5"/>
+    </row>
+    <row r="215" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D215" s="5"/>
+    </row>
+    <row r="216" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D216" s="5"/>
+    </row>
+    <row r="217" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D217" s="5"/>
+    </row>
+    <row r="218" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D218" s="5"/>
+    </row>
+    <row r="219" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D219" s="5"/>
+    </row>
+    <row r="220" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D220" s="5"/>
+    </row>
+    <row r="221" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D221" s="5"/>
+    </row>
+    <row r="222" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D222" s="5"/>
+    </row>
+    <row r="223" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D223" s="5"/>
+    </row>
+    <row r="224" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D224" s="5"/>
+    </row>
+    <row r="225" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D225" s="5"/>
+    </row>
+    <row r="226" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D226" s="5"/>
+    </row>
+    <row r="227" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D227" s="5"/>
+    </row>
+    <row r="228" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D228" s="5"/>
+    </row>
+    <row r="229" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D229" s="5"/>
+    </row>
+    <row r="230" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D230" s="5"/>
+    </row>
+    <row r="231" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D231" s="5"/>
+    </row>
+    <row r="232" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D232" s="5"/>
+    </row>
+    <row r="233" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D233" s="5"/>
+    </row>
+    <row r="234" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D234" s="5"/>
+    </row>
+    <row r="235" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D235" s="5"/>
+    </row>
+    <row r="236" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D236" s="5"/>
+    </row>
+    <row r="237" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D237" s="5"/>
+    </row>
+    <row r="238" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D238" s="5"/>
+    </row>
+    <row r="239" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D239" s="5"/>
+    </row>
+    <row r="240" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D240" s="5"/>
+    </row>
+    <row r="241" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D241" s="5"/>
+    </row>
+    <row r="242" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D242" s="5"/>
+    </row>
+    <row r="243" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D243" s="5"/>
+    </row>
+    <row r="244" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D244" s="5"/>
+    </row>
+    <row r="245" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D245" s="5"/>
+    </row>
+    <row r="246" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D246" s="5"/>
+    </row>
+    <row r="247" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D247" s="5"/>
+    </row>
+    <row r="248" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D248" s="5"/>
+    </row>
+    <row r="249" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D249" s="5"/>
+    </row>
+    <row r="250" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D250" s="5"/>
+    </row>
+    <row r="251" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D251" s="5"/>
+    </row>
+    <row r="252" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D252" s="5"/>
+    </row>
+    <row r="253" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D253" s="5"/>
+    </row>
+    <row r="254" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D254" s="5"/>
+    </row>
+    <row r="255" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D255" s="5"/>
+    </row>
+    <row r="256" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D256" s="5"/>
+    </row>
+    <row r="257" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D257" s="5"/>
+    </row>
+    <row r="258" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D258" s="5"/>
+    </row>
+    <row r="259" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D259" s="5"/>
+    </row>
+    <row r="260" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D260" s="5"/>
+    </row>
+    <row r="261" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D261" s="5"/>
+    </row>
+    <row r="262" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D262" s="5"/>
+    </row>
+    <row r="263" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D263" s="5"/>
+    </row>
+    <row r="264" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D264" s="5"/>
+    </row>
+    <row r="265" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D265" s="5"/>
+    </row>
+    <row r="266" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D266" s="5"/>
+    </row>
+    <row r="267" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D267" s="5"/>
+    </row>
+    <row r="268" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D268" s="5"/>
+    </row>
+    <row r="269" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D269" s="5"/>
+    </row>
+    <row r="270" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D270" s="5"/>
+    </row>
+    <row r="271" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D271" s="5"/>
+    </row>
+    <row r="272" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D272" s="5"/>
+    </row>
+    <row r="273" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D273" s="5"/>
+    </row>
+    <row r="274" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D274" s="5"/>
+    </row>
+    <row r="275" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D275" s="5"/>
+    </row>
+    <row r="276" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D276" s="5"/>
+    </row>
+    <row r="277" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D277" s="5"/>
+    </row>
+    <row r="278" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D278" s="5"/>
+    </row>
+    <row r="279" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D279" s="5"/>
+    </row>
+    <row r="280" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D280" s="5"/>
+    </row>
+    <row r="281" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D281" s="5"/>
+    </row>
+    <row r="282" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D282" s="5"/>
+    </row>
+    <row r="283" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D283" s="5"/>
+    </row>
+    <row r="284" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D284" s="5"/>
+    </row>
+    <row r="285" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D285" s="5"/>
+    </row>
+    <row r="286" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D286" s="5"/>
+    </row>
+    <row r="287" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D287" s="5"/>
+    </row>
+    <row r="288" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D288" s="5"/>
+    </row>
+    <row r="289" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D289" s="5"/>
+    </row>
+    <row r="290" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D290" s="5"/>
+    </row>
+    <row r="291" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D291" s="5"/>
+    </row>
+    <row r="292" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D292" s="5"/>
+    </row>
+    <row r="293" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D293" s="5"/>
+    </row>
+    <row r="294" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D294" s="5"/>
+    </row>
+    <row r="295" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D295" s="5"/>
+    </row>
+    <row r="296" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D296" s="5"/>
+    </row>
+    <row r="297" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D297" s="5"/>
+    </row>
+    <row r="298" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D298" s="5"/>
+    </row>
+    <row r="299" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D299" s="5"/>
+    </row>
+    <row r="300" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D300" s="5"/>
+    </row>
+    <row r="301" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D301" s="5"/>
+    </row>
+    <row r="302" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D302" s="5"/>
+    </row>
+    <row r="303" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D303" s="5"/>
+    </row>
+    <row r="304" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D304" s="5"/>
+    </row>
+    <row r="305" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D305" s="5"/>
+    </row>
+    <row r="306" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D306" s="5"/>
+    </row>
+    <row r="307" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D307" s="5"/>
+    </row>
+    <row r="308" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D308" s="5"/>
+    </row>
+    <row r="309" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D309" s="5"/>
+    </row>
+    <row r="310" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D310" s="5"/>
+    </row>
+    <row r="311" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D311" s="5"/>
+    </row>
+    <row r="312" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D312" s="5"/>
+    </row>
+    <row r="313" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D313" s="5"/>
+    </row>
+    <row r="314" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D314" s="5"/>
+    </row>
+    <row r="315" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D315" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FD18739-0A8F-2D47-A6B3-6B11335B6D41}">
+  <dimension ref="A1:D54"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="77.83203125" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" customWidth="1"/>
+    <col min="4" max="4" width="121.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="4"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="4"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="4"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="4"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="4"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="4"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="4"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="4"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="4"/>
+      <c r="B48" s="4"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="4"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="4"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="4"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="4"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="4"/>
+      <c r="D50" s="4"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="4"/>
+      <c r="B51" s="4"/>
+      <c r="C51" s="4"/>
+      <c r="D51" s="4"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="4"/>
+      <c r="B52" s="4"/>
+      <c r="C52" s="4"/>
+      <c r="D52" s="4"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="4"/>
+      <c r="B53" s="4"/>
+      <c r="C53" s="4"/>
+      <c r="D53" s="4"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="4"/>
+      <c r="B54" s="4"/>
+      <c r="C54" s="4"/>
+      <c r="D54" s="4"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>